<commit_message>
add test to select lotion type
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbamnote/eclipse-workspace/WeatherS/WeatherShopper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C8B874-78DC-1748-B2B1-F47BE157D3E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7249197A-4129-9C47-83C6-DCDEA965622F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Status" sheetId="2" r:id="rId1"/>
+    <sheet name="TestStatus" sheetId="2" r:id="rId1"/>
     <sheet name="TestCases" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>MoisturizerTest</t>
   </si>
@@ -73,9 +73,6 @@
     <t>SPF20</t>
   </si>
   <si>
-    <t>Cheap</t>
-  </si>
-  <si>
     <t>Expensive</t>
   </si>
   <si>
@@ -83,6 +80,15 @@
   </si>
   <si>
     <t>TCID</t>
+  </si>
+  <si>
+    <t>ProductTypeTest</t>
+  </si>
+  <si>
+    <t>Least</t>
+  </si>
+  <si>
+    <t>Almond</t>
   </si>
 </sst>
 </file>
@@ -98,7 +104,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +123,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -130,10 +142,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1969E6-80C9-B046-A5B1-C4973608F424}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,15 +475,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -477,9 +491,17 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -490,10 +512,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0485BAA-FADE-774F-BDC4-4EA3433A8408}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,8 +525,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -514,12 +536,6 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -528,44 +544,38 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
+      <c r="D7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -576,10 +586,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -590,10 +600,57 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add testcase to select moisturizer and add to the cart
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbamnote/eclipse-workspace/WeatherS/WeatherShopper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7249197A-4129-9C47-83C6-DCDEA965622F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8784A172-A2D3-F746-8D50-AD525D9A584C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>MoisturizerTest</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>ProductContent</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -58,37 +55,28 @@
     <t>Aloe</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Mozilla</t>
-  </si>
-  <si>
     <t>SunscreenTest</t>
   </si>
   <si>
-    <t>SPF50</t>
-  </si>
-  <si>
-    <t>SPF20</t>
-  </si>
-  <si>
-    <t>Expensive</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>TCID</t>
   </si>
   <si>
     <t>ProductTypeTest</t>
   </si>
   <si>
-    <t>Least</t>
+    <t>ProductContent1</t>
+  </si>
+  <si>
+    <t>ProductContent2</t>
   </si>
   <si>
     <t>Almond</t>
+  </si>
+  <si>
+    <t>SPF-50</t>
+  </si>
+  <si>
+    <t>SPF-30</t>
   </si>
 </sst>
 </file>
@@ -475,7 +463,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -483,10 +471,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -494,15 +482,15 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -512,21 +500,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0485BAA-FADE-774F-BDC4-4EA3433A8408}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -539,10 +527,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -558,99 +546,57 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="D11" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add logic to select sunscreen and add to the cart
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbamnote/eclipse-workspace/WeatherS/WeatherShopper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8784A172-A2D3-F746-8D50-AD525D9A584C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7792F9-7507-F941-8B66-85004C040A89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>MoisturizerTest</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>Aloe</t>
-  </si>
-  <si>
     <t>SunscreenTest</t>
   </si>
   <si>
@@ -70,13 +67,22 @@
     <t>ProductContent2</t>
   </si>
   <si>
-    <t>Almond</t>
-  </si>
-  <si>
     <t>SPF-50</t>
   </si>
   <si>
     <t>SPF-30</t>
+  </si>
+  <si>
+    <t>ALOE</t>
+  </si>
+  <si>
+    <t>ALMOND</t>
+  </si>
+  <si>
+    <t>ProductContent3</t>
+  </si>
+  <si>
+    <t>ProductContent4</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -471,7 +477,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -487,7 +493,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0485BAA-FADE-774F-BDC4-4EA3433A8408}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,12 +518,12 @@
     <col min="3" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -525,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -533,12 +539,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -546,13 +552,19 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -560,18 +572,24 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -579,13 +597,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -593,10 +611,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add card details and check payment status
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbamnote/eclipse-workspace/WeatherS/WeatherShopper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7792F9-7507-F941-8B66-85004C040A89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07055F93-589D-7B41-B44F-C85512B32F59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>MoisturizerTest</t>
   </si>
@@ -79,20 +79,55 @@
     <t>ALMOND</t>
   </si>
   <si>
-    <t>ProductContent3</t>
-  </si>
-  <si>
-    <t>ProductContent4</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>CCNumber</t>
+  </si>
+  <si>
+    <t>CCDate</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>swapbamnote@gmail.com</t>
+  </si>
+  <si>
+    <t>CCZipCode</t>
+  </si>
+  <si>
+    <t>4242424242424242</t>
+  </si>
+  <si>
+    <t>MoisturizerContent1</t>
+  </si>
+  <si>
+    <t>MoisturizerContent2</t>
+  </si>
+  <si>
+    <t>SunscreenContent1</t>
+  </si>
+  <si>
+    <t>SunscreenContent2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,17 +168,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,7 +546,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0485BAA-FADE-774F-BDC4-4EA3433A8408}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -516,14 +556,17 @@
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -531,7 +574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -539,12 +582,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -552,19 +595,34 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -583,13 +641,28 @@
       <c r="F7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1222</v>
+      </c>
+      <c r="J7" s="6">
+        <v>123</v>
+      </c>
+      <c r="K7" s="6">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -603,7 +676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -618,6 +691,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1" xr:uid="{9DB9B6C5-33A3-7247-ACBE-EC92EAF3B109}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test name modification in input file
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbamnote/eclipse-workspace/WeatherS/WeatherShopper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07055F93-589D-7B41-B44F-C85512B32F59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A78EA35-66C9-374E-B36B-BA70808065B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
-  <si>
-    <t>MoisturizerTest</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Runmode</t>
   </si>
@@ -52,21 +49,12 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>SunscreenTest</t>
-  </si>
-  <si>
     <t>TCID</t>
   </si>
   <si>
     <t>ProductTypeTest</t>
   </si>
   <si>
-    <t>ProductContent1</t>
-  </si>
-  <si>
-    <t>ProductContent2</t>
-  </si>
-  <si>
     <t>SPF-50</t>
   </si>
   <si>
@@ -110,6 +98,9 @@
   </si>
   <si>
     <t>SunscreenContent2</t>
+  </si>
+  <si>
+    <t>BuyBodyLotionTest</t>
   </si>
 </sst>
 </file>
@@ -496,7 +487,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1969E6-80C9-B046-A5B1-C4973608F424}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -504,39 +495,31 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -546,15 +529,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0485BAA-FADE-774F-BDC4-4EA3433A8408}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -563,89 +546,89 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I7" s="6">
         <v>1222</v>
@@ -655,39 +638,6 @@
       </c>
       <c r="K7" s="6">
         <v>12345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verify cart and total price
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbamnote/eclipse-workspace/WeatherS/WeatherShopper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE275995-2069-444F-A29F-13D124343E8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53AB058-98C7-B446-929B-074FEA3D895B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
   </bookViews>
@@ -576,7 +576,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
log result separately for each data
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbamnote/eclipse-workspace/WeatherS/WeatherShopper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1C55AC-AF12-5347-9581-BD6C0303FF80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EDE893-B44D-7747-8C73-4ACC4DB9067F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Runmode</t>
   </si>
@@ -97,16 +97,7 @@
     <t>BuyBodyLotionTest</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
     <t>chrome</t>
-  </si>
-  <si>
-    <t>safari</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>HomePageTest</t>
@@ -517,7 +508,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -538,9 +529,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0485BAA-FADE-774F-BDC4-4EA3433A8408}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -553,7 +546,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -569,63 +562,90 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>13</v>
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1222</v>
+      </c>
+      <c r="J8" s="6">
+        <v>123</v>
+      </c>
+      <c r="K8" s="6">
+        <v>12345</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -633,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -663,45 +683,10 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1222</v>
-      </c>
-      <c r="J10" s="6">
-        <v>123</v>
-      </c>
-      <c r="K10" s="6">
-        <v>12345</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G9" r:id="rId1" xr:uid="{9DB9B6C5-33A3-7247-ACBE-EC92EAF3B109}"/>
-    <hyperlink ref="G10" r:id="rId2" xr:uid="{53F2D156-22E3-DA4A-90E9-508161A82CDA}"/>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{9DB9B6C5-33A3-7247-ACBE-EC92EAF3B109}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{78D891ED-5A17-7D46-9019-AD15389F121D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
set execute listener to true before finding element
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbamnote/eclipse-workspace/WeatherS/WeatherShopper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EDE893-B44D-7747-8C73-4ACC4DB9067F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AB660E-94A9-9845-98DE-34F59AC1AA9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K9"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
different browsers as input and add comments
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbamnote/eclipse-workspace/WeatherS/WeatherShopper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AB660E-94A9-9845-98DE-34F59AC1AA9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C5A7CB-8311-4848-B389-8E08373B58DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{1083F305-AF86-9043-B75E-C4BAA06F7419}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Runmode</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>HomePageTest</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -653,7 +656,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>

</xml_diff>